<commit_message>
finale funktion angefangen (kampfablauf)
</commit_message>
<xml_diff>
--- a/data/held_margot.xlsx
+++ b/data/held_margot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E979ED-196A-407C-947C-4055178BB511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A8173D-9AA7-46E1-8416-060824953CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC708954-D5BA-48F4-A0A8-28752AA467BF}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>